<commit_message>
Cumprimento do requisito 3
</commit_message>
<xml_diff>
--- a/SpotifyClone-Non-NormalizedTable.xlsx
+++ b/SpotifyClone-Non-NormalizedTable.xlsx
@@ -31,24 +31,24 @@
     <t xml:space="preserve">idade</t>
   </si>
   <si>
+    <t xml:space="preserve">data_assinatura</t>
+  </si>
+  <si>
     <t xml:space="preserve">plano_id</t>
   </si>
   <si>
-    <t xml:space="preserve">data_assinatura</t>
-  </si>
-  <si>
     <t xml:space="preserve">PLANO</t>
   </si>
   <si>
     <t xml:space="preserve">Thati</t>
   </si>
   <si>
+    <t xml:space="preserve">2019-10-20</t>
+  </si>
+  <si>
     <t xml:space="preserve">1</t>
   </si>
   <si>
-    <t xml:space="preserve">2019-10-20</t>
-  </si>
-  <si>
     <t xml:space="preserve">name</t>
   </si>
   <si>
@@ -58,36 +58,36 @@
     <t xml:space="preserve">Cintia</t>
   </si>
   <si>
+    <t xml:space="preserve">2017-12-30</t>
+  </si>
+  <si>
     <t xml:space="preserve">2</t>
   </si>
   <si>
-    <t xml:space="preserve">2017-12-30</t>
-  </si>
-  <si>
     <t xml:space="preserve">gratuito</t>
   </si>
   <si>
     <t xml:space="preserve">Bill</t>
   </si>
   <si>
+    <t xml:space="preserve">2019-06-05</t>
+  </si>
+  <si>
     <t xml:space="preserve">3</t>
   </si>
   <si>
-    <t xml:space="preserve">2019-06-05</t>
-  </si>
-  <si>
     <t xml:space="preserve">familiar</t>
   </si>
   <si>
     <t xml:space="preserve">Roger</t>
   </si>
   <si>
+    <t xml:space="preserve">2020-05-13</t>
+  </si>
+  <si>
     <t xml:space="preserve">4</t>
   </si>
   <si>
-    <t xml:space="preserve">2020-05-13</t>
-  </si>
-  <si>
     <t xml:space="preserve">universitário</t>
   </si>
   <si>
@@ -148,12 +148,12 @@
     <t xml:space="preserve">album</t>
   </si>
   <si>
+    <t xml:space="preserve">ano_lancamento</t>
+  </si>
+  <si>
     <t xml:space="preserve">artista_id</t>
   </si>
   <si>
-    <t xml:space="preserve">ano_lancamento</t>
-  </si>
-  <si>
     <t xml:space="preserve">cancao_id</t>
   </si>
   <si>
@@ -247,10 +247,10 @@
     <t xml:space="preserve">Chained Down</t>
   </si>
   <si>
+    <t xml:space="preserve">2007</t>
+  </si>
+  <si>
     <t xml:space="preserve">5</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2007</t>
   </si>
   <si>
     <t xml:space="preserve">Honey, So Do I</t>
@@ -652,8 +652,8 @@
     <tableColumn id="1" name="id"/>
     <tableColumn id="2" name="usuario"/>
     <tableColumn id="3" name="idade"/>
-    <tableColumn id="4" name="plano_id"/>
-    <tableColumn id="5" name="data_assinatura"/>
+    <tableColumn id="4" name="data_assinatura"/>
+    <tableColumn id="5" name="plano_id"/>
   </tableColumns>
 </table>
 </file>
@@ -663,8 +663,8 @@
   <tableColumns count="6">
     <tableColumn id="1" name="album_id"/>
     <tableColumn id="2" name="album"/>
-    <tableColumn id="3" name="artista_id"/>
-    <tableColumn id="4" name="ano_lancamento"/>
+    <tableColumn id="3" name="ano_lancamento"/>
+    <tableColumn id="4" name="artista_id"/>
     <tableColumn id="5" name="Coluna5"/>
     <tableColumn id="6" name="cancao_id"/>
   </tableColumns>
@@ -687,8 +687,8 @@
   </sheetPr>
   <dimension ref="A1:Y999"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E19" activeCellId="0" sqref="E19"/>
+    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="J12" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="J25" activeCellId="0" sqref="J25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.5078125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -704,9 +704,9 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="20.5"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="8.83"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="21.47"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="23.67"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="22.86"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="0" width="8.83"/>
+    <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="13" min="13" style="0" width="23.67"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="11.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="0" width="23.79"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="0" width="18.8"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="0" width="15.67"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="18" style="0" width="14.28"/>
@@ -921,10 +921,10 @@
         <v>58</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="E6" s="5" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="F6" s="6"/>
       <c r="G6" s="12" t="n">
@@ -961,10 +961,10 @@
         <v>33</v>
       </c>
       <c r="D7" s="10" t="s">
-        <v>12</v>
+        <v>27</v>
       </c>
       <c r="E7" s="10" t="s">
-        <v>27</v>
+        <v>13</v>
       </c>
       <c r="F7" s="6"/>
       <c r="J7" s="8"/>
@@ -995,10 +995,10 @@
         <v>26</v>
       </c>
       <c r="D8" s="5" t="s">
-        <v>16</v>
+        <v>29</v>
       </c>
       <c r="E8" s="5" t="s">
-        <v>29</v>
+        <v>17</v>
       </c>
       <c r="F8" s="6"/>
       <c r="J8" s="8"/>
@@ -1029,10 +1029,10 @@
         <v>19</v>
       </c>
       <c r="D9" s="10" t="s">
-        <v>16</v>
+        <v>31</v>
       </c>
       <c r="E9" s="10" t="s">
-        <v>31</v>
+        <v>17</v>
       </c>
       <c r="F9" s="6"/>
       <c r="J9" s="8"/>
@@ -1063,10 +1063,10 @@
         <v>42</v>
       </c>
       <c r="D10" s="5" t="s">
-        <v>12</v>
+        <v>33</v>
       </c>
       <c r="E10" s="5" t="s">
-        <v>33</v>
+        <v>13</v>
       </c>
       <c r="F10" s="6"/>
       <c r="J10" s="8"/>
@@ -1097,10 +1097,10 @@
         <v>46</v>
       </c>
       <c r="D11" s="10" t="s">
-        <v>12</v>
+        <v>35</v>
       </c>
       <c r="E11" s="10" t="s">
-        <v>35</v>
+        <v>13</v>
       </c>
       <c r="F11" s="6"/>
       <c r="J11" s="8"/>
@@ -1180,10 +1180,10 @@
       <c r="B14" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="C14" s="1" t="s">
+      <c r="C14" s="14" t="s">
         <v>42</v>
       </c>
-      <c r="D14" s="14" t="s">
+      <c r="D14" s="1" t="s">
         <v>43</v>
       </c>
       <c r="F14" s="1" t="s">
@@ -1209,10 +1209,10 @@
         <v>45</v>
       </c>
       <c r="N14" s="14" t="s">
+        <v>40</v>
+      </c>
+      <c r="O14" s="14" t="s">
         <v>49</v>
-      </c>
-      <c r="O14" s="14" t="s">
-        <v>40</v>
       </c>
       <c r="Q14" s="7" t="s">
         <v>0</v>
@@ -1221,7 +1221,7 @@
         <v>48</v>
       </c>
       <c r="S14" s="7" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="T14" s="8"/>
     </row>
@@ -1232,11 +1232,11 @@
       <c r="B15" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="C15" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="D15" s="16" t="s">
+      <c r="C15" s="16" t="s">
         <v>51</v>
+      </c>
+      <c r="D15" s="5" t="s">
+        <v>8</v>
       </c>
       <c r="F15" s="4" t="n">
         <v>1</v>
@@ -1255,16 +1255,16 @@
         <v>1</v>
       </c>
       <c r="L15" s="16" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="M15" s="16" t="s">
         <v>53</v>
       </c>
-      <c r="N15" s="17" t="n">
+      <c r="N15" s="16" t="n">
+        <v>36</v>
+      </c>
+      <c r="O15" s="17" t="n">
         <v>43889.4485532407</v>
-      </c>
-      <c r="O15" s="16" t="n">
-        <v>36</v>
       </c>
       <c r="Q15" s="11" t="n">
         <v>1</v>
@@ -1273,7 +1273,7 @@
         <v>1</v>
       </c>
       <c r="S15" s="16" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="T15" s="8"/>
     </row>
@@ -1284,11 +1284,11 @@
       <c r="B16" s="10" t="s">
         <v>54</v>
       </c>
-      <c r="C16" s="10" t="s">
-        <v>7</v>
-      </c>
-      <c r="D16" s="18" t="s">
+      <c r="C16" s="18" t="s">
         <v>55</v>
+      </c>
+      <c r="D16" s="10" t="s">
+        <v>8</v>
       </c>
       <c r="F16" s="9" t="n">
         <v>2</v>
@@ -1312,11 +1312,11 @@
       <c r="M16" s="9" t="s">
         <v>57</v>
       </c>
-      <c r="N16" s="19" t="n">
+      <c r="N16" s="9" t="n">
+        <v>25</v>
+      </c>
+      <c r="O16" s="19" t="n">
         <v>43953.2295717593</v>
-      </c>
-      <c r="O16" s="9" t="n">
-        <v>25</v>
       </c>
       <c r="Q16" s="12" t="n">
         <v>2</v>
@@ -1325,7 +1325,7 @@
         <v>1</v>
       </c>
       <c r="S16" s="12" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="22.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1335,11 +1335,11 @@
       <c r="B17" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="C17" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="D17" s="16" t="s">
+      <c r="C17" s="16" t="s">
         <v>59</v>
+      </c>
+      <c r="D17" s="5" t="s">
+        <v>13</v>
       </c>
       <c r="F17" s="4" t="n">
         <v>3</v>
@@ -1363,11 +1363,11 @@
       <c r="M17" s="16" t="s">
         <v>61</v>
       </c>
-      <c r="N17" s="17" t="n">
+      <c r="N17" s="16" t="n">
+        <v>23</v>
+      </c>
+      <c r="O17" s="17" t="n">
         <v>43896.4739930556</v>
-      </c>
-      <c r="O17" s="16" t="n">
-        <v>23</v>
       </c>
       <c r="Q17" s="11" t="n">
         <v>3</v>
@@ -1376,7 +1376,7 @@
         <v>1</v>
       </c>
       <c r="S17" s="16" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="22.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1386,11 +1386,11 @@
       <c r="B18" s="10" t="s">
         <v>62</v>
       </c>
-      <c r="C18" s="10" t="s">
-        <v>16</v>
-      </c>
-      <c r="D18" s="18" t="s">
+      <c r="C18" s="18" t="s">
         <v>63</v>
+      </c>
+      <c r="D18" s="10" t="s">
+        <v>17</v>
       </c>
       <c r="F18" s="9" t="n">
         <v>4</v>
@@ -1414,11 +1414,11 @@
       <c r="M18" s="9" t="s">
         <v>65</v>
       </c>
-      <c r="N18" s="19" t="n">
+      <c r="N18" s="9" t="n">
+        <v>14</v>
+      </c>
+      <c r="O18" s="19" t="n">
         <v>44048.3370023148</v>
-      </c>
-      <c r="O18" s="9" t="n">
-        <v>14</v>
       </c>
       <c r="Q18" s="12" t="n">
         <v>4</v>
@@ -1427,7 +1427,7 @@
         <v>2</v>
       </c>
       <c r="S18" s="18" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="22.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1437,11 +1437,11 @@
       <c r="B19" s="5" t="s">
         <v>66</v>
       </c>
-      <c r="C19" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="D19" s="16" t="s">
+      <c r="C19" s="16" t="s">
         <v>67</v>
+      </c>
+      <c r="D19" s="5" t="s">
+        <v>21</v>
       </c>
       <c r="F19" s="4" t="n">
         <v>5</v>
@@ -1465,11 +1465,11 @@
       <c r="M19" s="16" t="s">
         <v>69</v>
       </c>
-      <c r="N19" s="17" t="n">
+      <c r="N19" s="16" t="n">
+        <v>15</v>
+      </c>
+      <c r="O19" s="17" t="n">
         <v>44088.6891435185</v>
-      </c>
-      <c r="O19" s="16" t="n">
-        <v>15</v>
       </c>
       <c r="Q19" s="11" t="n">
         <v>5</v>
@@ -1478,7 +1478,7 @@
         <v>2</v>
       </c>
       <c r="S19" s="16" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="22.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1488,11 +1488,11 @@
       <c r="B20" s="10" t="s">
         <v>70</v>
       </c>
-      <c r="C20" s="10" t="s">
-        <v>20</v>
-      </c>
-      <c r="D20" s="18" t="s">
+      <c r="C20" s="18" t="s">
         <v>71</v>
+      </c>
+      <c r="D20" s="10" t="s">
+        <v>21</v>
       </c>
       <c r="F20" s="9" t="n">
         <v>6</v>
@@ -1516,11 +1516,11 @@
       <c r="M20" s="9" t="s">
         <v>73</v>
       </c>
-      <c r="N20" s="19" t="n">
+      <c r="N20" s="9" t="n">
+        <v>34</v>
+      </c>
+      <c r="O20" s="19" t="n">
         <v>43832.3198263889</v>
-      </c>
-      <c r="O20" s="9" t="n">
-        <v>34</v>
       </c>
       <c r="Q20" s="12" t="n">
         <v>6</v>
@@ -1529,7 +1529,7 @@
         <v>3</v>
       </c>
       <c r="S20" s="18" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="22.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1539,10 +1539,10 @@
       <c r="B21" s="5" t="s">
         <v>74</v>
       </c>
-      <c r="C21" s="5" t="s">
+      <c r="C21" s="16" t="s">
         <v>75</v>
       </c>
-      <c r="D21" s="16" t="s">
+      <c r="D21" s="5" t="s">
         <v>76</v>
       </c>
       <c r="F21" s="4" t="n">
@@ -1567,11 +1567,11 @@
       <c r="M21" s="16" t="s">
         <v>78</v>
       </c>
-      <c r="N21" s="17" t="n">
+      <c r="N21" s="16" t="n">
+        <v>24</v>
+      </c>
+      <c r="O21" s="17" t="n">
         <v>43967.2613657407</v>
-      </c>
-      <c r="O21" s="16" t="n">
-        <v>24</v>
       </c>
       <c r="Q21" s="11" t="n">
         <v>7</v>
@@ -1580,7 +1580,7 @@
         <v>3</v>
       </c>
       <c r="S21" s="16" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="22.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1590,11 +1590,11 @@
       <c r="B22" s="10" t="s">
         <v>79</v>
       </c>
-      <c r="C22" s="10" t="s">
-        <v>75</v>
-      </c>
-      <c r="D22" s="18" t="s">
+      <c r="C22" s="18" t="s">
         <v>80</v>
+      </c>
+      <c r="D22" s="10" t="s">
+        <v>76</v>
       </c>
       <c r="F22" s="9" t="n">
         <v>8</v>
@@ -1618,11 +1618,11 @@
       <c r="M22" s="9" t="s">
         <v>82</v>
       </c>
-      <c r="N22" s="19" t="n">
+      <c r="N22" s="9" t="n">
+        <v>21</v>
+      </c>
+      <c r="O22" s="19" t="n">
         <v>44113.5193055556</v>
-      </c>
-      <c r="O22" s="9" t="n">
-        <v>21</v>
       </c>
       <c r="Q22" s="12" t="n">
         <v>8</v>
@@ -1631,7 +1631,7 @@
         <v>4</v>
       </c>
       <c r="S22" s="18" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="22.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1641,11 +1641,11 @@
       <c r="B23" s="5" t="s">
         <v>83</v>
       </c>
-      <c r="C23" s="5" t="s">
-        <v>75</v>
-      </c>
-      <c r="D23" s="16" t="s">
+      <c r="C23" s="16" t="s">
         <v>84</v>
+      </c>
+      <c r="D23" s="5" t="s">
+        <v>76</v>
       </c>
       <c r="F23" s="4" t="n">
         <v>9</v>
@@ -1669,11 +1669,11 @@
       <c r="M23" s="16" t="s">
         <v>86</v>
       </c>
-      <c r="N23" s="17" t="n">
+      <c r="N23" s="16" t="n">
+        <v>39</v>
+      </c>
+      <c r="O23" s="17" t="n">
         <v>44095.5519212963</v>
-      </c>
-      <c r="O23" s="16" t="n">
-        <v>39</v>
       </c>
       <c r="Q23" s="11" t="n">
         <v>9</v>
@@ -1682,7 +1682,7 @@
         <v>5</v>
       </c>
       <c r="S23" s="16" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="22.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1692,11 +1692,11 @@
       <c r="B24" s="10" t="s">
         <v>87</v>
       </c>
-      <c r="C24" s="10" t="s">
+      <c r="C24" s="18" t="s">
+        <v>84</v>
+      </c>
+      <c r="D24" s="10" t="s">
         <v>88</v>
-      </c>
-      <c r="D24" s="18" t="s">
-        <v>84</v>
       </c>
       <c r="F24" s="9" t="n">
         <v>10</v>
@@ -1720,11 +1720,11 @@
       <c r="M24" s="9" t="s">
         <v>72</v>
       </c>
-      <c r="N24" s="19" t="n">
+      <c r="N24" s="9" t="n">
+        <v>6</v>
+      </c>
+      <c r="O24" s="19" t="n">
         <v>44148.7050115741</v>
-      </c>
-      <c r="O24" s="9" t="n">
-        <v>6</v>
       </c>
       <c r="Q24" s="12" t="n">
         <v>10</v>
@@ -1769,11 +1769,11 @@
       <c r="M25" s="16" t="s">
         <v>60</v>
       </c>
-      <c r="N25" s="17" t="n">
+      <c r="N25" s="16" t="n">
+        <v>3</v>
+      </c>
+      <c r="O25" s="17" t="n">
         <v>44170.7767361111</v>
-      </c>
-      <c r="O25" s="16" t="n">
-        <v>3</v>
       </c>
       <c r="Q25" s="11" t="n">
         <v>11</v>
@@ -1818,11 +1818,11 @@
       <c r="M26" s="9" t="s">
         <v>93</v>
       </c>
-      <c r="N26" s="19" t="n">
+      <c r="N26" s="9" t="n">
+        <v>26</v>
+      </c>
+      <c r="O26" s="19" t="n">
         <v>44042.4166666667</v>
-      </c>
-      <c r="O26" s="9" t="n">
-        <v>26</v>
       </c>
       <c r="Q26" s="12" t="n">
         <v>12</v>
@@ -1831,7 +1831,7 @@
         <v>6</v>
       </c>
       <c r="S26" s="18" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="U26" s="8"/>
       <c r="V26" s="8"/>
@@ -1841,7 +1841,7 @@
     </row>
     <row r="27" customFormat="false" ht="22.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A27" s="7" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B27" s="7" t="s">
         <v>94</v>
@@ -1869,11 +1869,11 @@
       <c r="M27" s="16" t="s">
         <v>56</v>
       </c>
-      <c r="N27" s="17" t="n">
+      <c r="N27" s="16" t="n">
+        <v>2</v>
+      </c>
+      <c r="O27" s="17" t="n">
         <v>44423.7153935185</v>
-      </c>
-      <c r="O27" s="16" t="n">
-        <v>2</v>
       </c>
       <c r="Q27" s="11" t="n">
         <v>13</v>
@@ -1882,7 +1882,7 @@
         <v>6</v>
       </c>
       <c r="S27" s="16" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="U27" s="8"/>
       <c r="V27" s="8"/>
@@ -1920,11 +1920,11 @@
       <c r="M28" s="9" t="s">
         <v>97</v>
       </c>
-      <c r="N28" s="19" t="n">
+      <c r="N28" s="9" t="n">
+        <v>35</v>
+      </c>
+      <c r="O28" s="19" t="n">
         <v>44387.6392361111</v>
-      </c>
-      <c r="O28" s="9" t="n">
-        <v>35</v>
       </c>
       <c r="Q28" s="12" t="n">
         <v>14</v>
@@ -1933,7 +1933,7 @@
         <v>7</v>
       </c>
       <c r="S28" s="18" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="U28" s="8"/>
       <c r="V28" s="8"/>
@@ -1971,11 +1971,11 @@
       <c r="M29" s="16" t="s">
         <v>99</v>
       </c>
-      <c r="N29" s="17" t="n">
+      <c r="N29" s="16" t="n">
+        <v>27</v>
+      </c>
+      <c r="O29" s="17" t="n">
         <v>44205.0726041667</v>
-      </c>
-      <c r="O29" s="16" t="n">
-        <v>27</v>
       </c>
       <c r="Q29" s="11" t="n">
         <v>15</v>
@@ -1984,7 +1984,7 @@
         <v>7</v>
       </c>
       <c r="S29" s="16" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="U29" s="8"/>
       <c r="V29" s="8"/>
@@ -2022,11 +2022,11 @@
       <c r="M30" s="9" t="s">
         <v>77</v>
       </c>
-      <c r="N30" s="19" t="n">
+      <c r="N30" s="9" t="n">
+        <v>7</v>
+      </c>
+      <c r="O30" s="19" t="n">
         <v>44015.8149074074</v>
-      </c>
-      <c r="O30" s="9" t="n">
-        <v>7</v>
       </c>
       <c r="Q30" s="12" t="n">
         <v>16</v>
@@ -2035,7 +2035,7 @@
         <v>8</v>
       </c>
       <c r="S30" s="18" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="U30" s="8"/>
       <c r="V30" s="8"/>
@@ -2073,11 +2073,11 @@
       <c r="M31" s="16" t="s">
         <v>92</v>
       </c>
-      <c r="N31" s="17" t="n">
+      <c r="N31" s="16" t="n">
+        <v>12</v>
+      </c>
+      <c r="O31" s="17" t="n">
         <v>42790.8849768519</v>
-      </c>
-      <c r="O31" s="16" t="n">
-        <v>12</v>
       </c>
       <c r="Q31" s="11" t="n">
         <v>17</v>
@@ -2086,7 +2086,7 @@
         <v>8</v>
       </c>
       <c r="S31" s="16" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="U31" s="8"/>
       <c r="V31" s="8"/>
@@ -2124,11 +2124,11 @@
       <c r="M32" s="9" t="s">
         <v>65</v>
       </c>
-      <c r="N32" s="19" t="n">
+      <c r="N32" s="9" t="n">
+        <v>14</v>
+      </c>
+      <c r="O32" s="19" t="n">
         <v>44049.6414699074</v>
-      </c>
-      <c r="O32" s="9" t="n">
-        <v>14</v>
       </c>
       <c r="Q32" s="12" t="n">
         <v>18</v>
@@ -2175,11 +2175,11 @@
       <c r="M33" s="16" t="s">
         <v>52</v>
       </c>
-      <c r="N33" s="17" t="n">
+      <c r="N33" s="16" t="n">
+        <v>1</v>
+      </c>
+      <c r="O33" s="17" t="n">
         <v>44145.5780902778</v>
-      </c>
-      <c r="O33" s="16" t="n">
-        <v>1</v>
       </c>
       <c r="Q33" s="11" t="n">
         <v>19</v>
@@ -2188,7 +2188,7 @@
         <v>9</v>
       </c>
       <c r="S33" s="16" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="U33" s="8"/>
       <c r="V33" s="8"/>
@@ -2222,11 +2222,11 @@
       <c r="M34" s="9" t="s">
         <v>109</v>
       </c>
-      <c r="N34" s="19" t="n">
+      <c r="N34" s="9" t="n">
+        <v>38</v>
+      </c>
+      <c r="O34" s="19" t="n">
         <v>43503.8568055556</v>
-      </c>
-      <c r="O34" s="9" t="n">
-        <v>38</v>
       </c>
       <c r="Q34" s="12" t="n">
         <v>20</v>
@@ -2235,7 +2235,7 @@
         <v>9</v>
       </c>
       <c r="S34" s="18" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="U34" s="8"/>
       <c r="V34" s="8"/>
@@ -2267,11 +2267,11 @@
       <c r="M35" s="16" t="s">
         <v>110</v>
       </c>
-      <c r="N35" s="17" t="n">
+      <c r="N35" s="16" t="n">
+        <v>29</v>
+      </c>
+      <c r="O35" s="17" t="n">
         <v>42759.021724537</v>
-      </c>
-      <c r="O35" s="16" t="n">
-        <v>29</v>
       </c>
       <c r="Q35" s="11" t="n">
         <v>21</v>
@@ -2280,7 +2280,7 @@
         <v>10</v>
       </c>
       <c r="S35" s="16" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="U35" s="8"/>
       <c r="V35" s="8"/>
@@ -2312,11 +2312,11 @@
       <c r="M36" s="9" t="s">
         <v>112</v>
       </c>
-      <c r="N36" s="19" t="n">
+      <c r="N36" s="9" t="n">
+        <v>30</v>
+      </c>
+      <c r="O36" s="19" t="n">
         <v>43020.524537037</v>
-      </c>
-      <c r="O36" s="9" t="n">
-        <v>30</v>
       </c>
       <c r="Q36" s="12" t="n">
         <v>22</v>
@@ -2359,11 +2359,11 @@
       <c r="M37" s="16" t="s">
         <v>111</v>
       </c>
-      <c r="N37" s="17" t="n">
+      <c r="N37" s="16" t="n">
+        <v>22</v>
+      </c>
+      <c r="O37" s="17" t="n">
         <v>43249.6226967593</v>
-      </c>
-      <c r="O37" s="16" t="n">
-        <v>22</v>
       </c>
       <c r="R37" s="8"/>
       <c r="S37" s="8"/>
@@ -2399,11 +2399,11 @@
       <c r="M38" s="9" t="s">
         <v>68</v>
       </c>
-      <c r="N38" s="19" t="n">
+      <c r="N38" s="9" t="n">
+        <v>5</v>
+      </c>
+      <c r="O38" s="19" t="n">
         <v>43229.9380671296</v>
-      </c>
-      <c r="O38" s="9" t="n">
-        <v>5</v>
       </c>
       <c r="R38" s="8"/>
       <c r="S38" s="8"/>
@@ -2439,11 +2439,11 @@
       <c r="M39" s="16" t="s">
         <v>64</v>
       </c>
-      <c r="N39" s="17" t="n">
+      <c r="N39" s="16" t="n">
+        <v>4</v>
+      </c>
+      <c r="O39" s="17" t="n">
         <v>44039.5367824074</v>
-      </c>
-      <c r="O39" s="16" t="n">
-        <v>4</v>
       </c>
       <c r="P39" s="8"/>
       <c r="Q39" s="8"/>
@@ -2481,11 +2481,11 @@
       <c r="M40" s="9" t="s">
         <v>90</v>
       </c>
-      <c r="N40" s="19" t="n">
+      <c r="N40" s="9" t="n">
+        <v>11</v>
+      </c>
+      <c r="O40" s="19" t="n">
         <v>43116.778275463</v>
-      </c>
-      <c r="O40" s="9" t="n">
-        <v>11</v>
       </c>
       <c r="P40" s="8"/>
       <c r="Q40" s="8"/>
@@ -2523,11 +2523,11 @@
       <c r="M41" s="16" t="s">
         <v>86</v>
       </c>
-      <c r="N41" s="17" t="n">
+      <c r="N41" s="16" t="n">
+        <v>39</v>
+      </c>
+      <c r="O41" s="17" t="n">
         <v>43180.7060185185</v>
-      </c>
-      <c r="O41" s="16" t="n">
-        <v>39</v>
       </c>
       <c r="P41" s="8"/>
       <c r="Q41" s="8"/>
@@ -2565,11 +2565,11 @@
       <c r="M42" s="9" t="s">
         <v>114</v>
       </c>
-      <c r="N42" s="19" t="n">
+      <c r="N42" s="9" t="n">
+        <v>40</v>
+      </c>
+      <c r="O42" s="19" t="n">
         <v>44122.5681134259</v>
-      </c>
-      <c r="O42" s="9" t="n">
-        <v>40</v>
       </c>
       <c r="P42" s="8"/>
       <c r="Q42" s="8"/>
@@ -2607,11 +2607,11 @@
       <c r="M43" s="16" t="s">
         <v>115</v>
       </c>
-      <c r="N43" s="17" t="n">
+      <c r="N43" s="16" t="n">
+        <v>32</v>
+      </c>
+      <c r="O43" s="17" t="n">
         <v>43610.3430902778</v>
-      </c>
-      <c r="O43" s="16" t="n">
-        <v>32</v>
       </c>
       <c r="P43" s="8"/>
       <c r="Q43" s="8"/>
@@ -2649,11 +2649,11 @@
       <c r="M44" s="9" t="s">
         <v>116</v>
       </c>
-      <c r="N44" s="19" t="n">
+      <c r="N44" s="9" t="n">
+        <v>33</v>
+      </c>
+      <c r="O44" s="19" t="n">
         <v>44423.9007986111</v>
-      </c>
-      <c r="O44" s="9" t="n">
-        <v>33</v>
       </c>
       <c r="P44" s="8"/>
       <c r="Q44" s="8"/>
@@ -2691,11 +2691,11 @@
       <c r="M45" s="16" t="s">
         <v>101</v>
       </c>
-      <c r="N45" s="17" t="n">
+      <c r="N45" s="16" t="n">
+        <v>16</v>
+      </c>
+      <c r="O45" s="17" t="n">
         <v>44340.7248263889</v>
-      </c>
-      <c r="O45" s="16" t="n">
-        <v>16</v>
       </c>
       <c r="P45" s="8"/>
       <c r="Q45" s="8"/>
@@ -2733,11 +2733,11 @@
       <c r="M46" s="9" t="s">
         <v>103</v>
       </c>
-      <c r="N46" s="19" t="n">
+      <c r="N46" s="9" t="n">
+        <v>17</v>
+      </c>
+      <c r="O46" s="19" t="n">
         <v>43441.9506018519</v>
-      </c>
-      <c r="O46" s="9" t="n">
-        <v>17</v>
       </c>
       <c r="P46" s="8"/>
       <c r="Q46" s="8"/>
@@ -2775,11 +2775,11 @@
       <c r="M47" s="16" t="s">
         <v>81</v>
       </c>
-      <c r="N47" s="17" t="n">
+      <c r="N47" s="16" t="n">
+        <v>8</v>
+      </c>
+      <c r="O47" s="17" t="n">
         <v>44269.2600231482</v>
-      </c>
-      <c r="O47" s="16" t="n">
-        <v>8</v>
       </c>
       <c r="P47" s="8"/>
       <c r="Q47" s="8"/>
@@ -2817,11 +2817,11 @@
       <c r="M48" s="9" t="s">
         <v>85</v>
       </c>
-      <c r="N48" s="19" t="n">
+      <c r="N48" s="9" t="n">
+        <v>9</v>
+      </c>
+      <c r="O48" s="19" t="n">
         <v>43922.15</v>
-      </c>
-      <c r="O48" s="9" t="n">
-        <v>9</v>
       </c>
       <c r="P48" s="8"/>
       <c r="Q48" s="8"/>
@@ -2859,11 +2859,11 @@
       <c r="M49" s="16" t="s">
         <v>108</v>
       </c>
-      <c r="N49" s="17" t="n">
+      <c r="N49" s="16" t="n">
+        <v>20</v>
+      </c>
+      <c r="O49" s="17" t="n">
         <v>42772.3483101852</v>
-      </c>
-      <c r="O49" s="16" t="n">
-        <v>20</v>
       </c>
       <c r="P49" s="8"/>
       <c r="Q49" s="8"/>
@@ -2901,11 +2901,11 @@
       <c r="M50" s="9" t="s">
         <v>82</v>
       </c>
-      <c r="N50" s="19" t="n">
+      <c r="N50" s="9" t="n">
+        <v>21</v>
+      </c>
+      <c r="O50" s="19" t="n">
         <v>43073.2317476852</v>
-      </c>
-      <c r="O50" s="9" t="n">
-        <v>21</v>
       </c>
       <c r="P50" s="8"/>
       <c r="Q50" s="8"/>
@@ -2943,11 +2943,11 @@
       <c r="M51" s="16" t="s">
         <v>92</v>
       </c>
-      <c r="N51" s="17" t="n">
+      <c r="N51" s="16" t="n">
+        <v>12</v>
+      </c>
+      <c r="O51" s="17" t="n">
         <v>42943.2255671296</v>
-      </c>
-      <c r="O51" s="16" t="n">
-        <v>12</v>
       </c>
       <c r="P51" s="8"/>
       <c r="Q51" s="8"/>
@@ -2985,11 +2985,11 @@
       <c r="M52" s="9" t="s">
         <v>95</v>
       </c>
-      <c r="N52" s="19" t="n">
+      <c r="N52" s="9" t="n">
+        <v>13</v>
+      </c>
+      <c r="O52" s="19" t="n">
         <v>43094.0444097222</v>
-      </c>
-      <c r="O52" s="9" t="n">
-        <v>13</v>
       </c>
       <c r="P52" s="8"/>
       <c r="Q52" s="8"/>

</xml_diff>